<commit_message>
fixed some inconsistencies in bom
</commit_message>
<xml_diff>
--- a/slave_bom.xlsx
+++ b/slave_bom.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="246">
   <si>
     <t>Qty</t>
   </si>
@@ -169,9 +169,6 @@
     <t>1,00µF Keramik-Kondensator</t>
   </si>
   <si>
-    <t>24AA02UID</t>
-  </si>
-  <si>
     <t>3.3k, 10%, 1/10W</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>3,30K SMD - CHIP - Dickschichtwiderstand</t>
   </si>
   <si>
-    <t>4.7k, 10%, 1/10W</t>
-  </si>
-  <si>
     <t>43045-0200_MOLEX_2PIN</t>
   </si>
   <si>
@@ -220,15 +214,9 @@
     <t>MMSZ4xxxT1G Serie - ON Semiconductor</t>
   </si>
   <si>
-    <t>75R, 10%, 0.4W</t>
-  </si>
-  <si>
     <t>R_SMD_2010_R_YAGEO_REV01</t>
   </si>
   <si>
-    <t>806, 1%, 1/10W</t>
-  </si>
-  <si>
     <t>820R_0603_R_VISHAY_1%_TK100_REV_01</t>
   </si>
   <si>
@@ -283,9 +271,6 @@
     <t>HX1188NL</t>
   </si>
   <si>
-    <t>LTC1380CGN</t>
-  </si>
-  <si>
     <t>LTC6255CS6</t>
   </si>
   <si>
@@ -340,9 +325,6 @@
     <t>PBHV8115Z - NXP</t>
   </si>
   <si>
-    <t>PCF8574TS/3</t>
-  </si>
-  <si>
     <t>SOP65P640X150-20N</t>
   </si>
   <si>
@@ -694,9 +676,6 @@
     <t>R813, R901, R902, R903, R904, R905, R906, R907, R908, R1001, R1002, R1003, R1004, R1005, R1006, R1007, R1008, R1101, R1102, R1103, R1104, R1105, R1106, R1107, R1108, R1201, R1202, R1203, R1204, R1205, R1206, R1207, R1208, R1301, R1401, R1606</t>
   </si>
   <si>
-    <t>402K_0603_R_VISHAY_1%_TK100_REV_01</t>
-  </si>
-  <si>
     <t>R1601</t>
   </si>
   <si>
@@ -761,6 +740,18 @@
   </si>
   <si>
     <t>270R_0603_R_VISHAY_1%_TK100_REV_01</t>
+  </si>
+  <si>
+    <t>270R, 10%, 1/10W</t>
+  </si>
+  <si>
+    <t>1.2k, 10%, 1/10W</t>
+  </si>
+  <si>
+    <t>68R, 10%, 0.4W</t>
+  </si>
+  <si>
+    <t>820R, 1%, 1/10W</t>
   </si>
 </sst>
 </file>
@@ -1781,7 +1772,7 @@
   <cols>
     <col min="1" max="1" width="11.42578125" style="4"/>
     <col min="2" max="2" width="13.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="34.140625" customWidth="1"/>
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="50.7109375" customWidth="1"/>
@@ -1798,7 +1789,7 @@
   <sheetData>
     <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -1848,7 +1839,7 @@
     <row r="3" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A3" s="11"/>
       <c r="B3" s="13" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -1876,7 +1867,7 @@
         <v>12</v>
       </c>
       <c r="F4" s="24" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="G4" s="23" t="s">
         <v>13</v>
@@ -1909,7 +1900,7 @@
         <v>12</v>
       </c>
       <c r="F5" s="24" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="G5" s="23" t="s">
         <v>19</v>
@@ -1943,7 +1934,7 @@
         <v>12</v>
       </c>
       <c r="F6" s="24" t="s">
-        <v>225</v>
+        <v>219</v>
       </c>
       <c r="G6" s="23" t="s">
         <v>21</v>
@@ -1977,7 +1968,7 @@
         <v>26</v>
       </c>
       <c r="F7" s="24" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G7" s="23" t="s">
         <v>24</v>
@@ -2011,7 +2002,7 @@
         <v>12</v>
       </c>
       <c r="F8" s="24" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="G8" s="23" t="s">
         <v>24</v>
@@ -2045,7 +2036,7 @@
         <v>12</v>
       </c>
       <c r="F9" s="24" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="G9" s="23" t="s">
         <v>42</v>
@@ -2079,7 +2070,7 @@
         <v>12</v>
       </c>
       <c r="F10" s="24" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="G10" s="23" t="s">
         <v>44</v>
@@ -2113,7 +2104,7 @@
         <v>12</v>
       </c>
       <c r="F11" s="24" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="G11" s="23" t="s">
         <v>47</v>
@@ -2138,19 +2129,19 @@
         <v>2</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>45</v>
+        <v>242</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F12" s="24" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G12" s="23" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="H12" s="19">
         <v>2141320</v>
@@ -2172,19 +2163,19 @@
         <v>12</v>
       </c>
       <c r="C13" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="23" t="s">
         <v>52</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>53</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="24" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G13" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H13" s="19">
         <v>1469793</v>
@@ -2200,25 +2191,25 @@
     </row>
     <row r="14" spans="1:57" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="21" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="B14" s="19">
         <v>4</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>55</v>
+        <v>243</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F14" s="24" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="G14" s="23" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="H14" s="19">
         <v>1469741</v>
@@ -2234,25 +2225,25 @@
     </row>
     <row r="15" spans="1:57" s="25" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="B15" s="19">
         <v>24</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>68</v>
+        <v>244</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="E15" s="23" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F15" s="24" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G15" s="23" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="H15" s="19">
         <v>2323988</v>
@@ -2274,19 +2265,19 @@
         <v>2</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>70</v>
+        <v>245</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F16" s="24" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="H16" s="19">
         <v>1469841</v>
@@ -2308,19 +2299,19 @@
         <v>1</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F17" s="23" t="s">
-        <v>227</v>
+        <v>220</v>
       </c>
       <c r="G17" s="23" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="H17" s="19">
         <v>2303278</v>
@@ -2341,19 +2332,19 @@
         <v>1</v>
       </c>
       <c r="C18" s="23" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D18" s="23" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="E18" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="23" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="G18" s="23" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="H18" s="19">
         <v>2059490</v>
@@ -2374,19 +2365,19 @@
         <v>1</v>
       </c>
       <c r="C19" s="23" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="D19" s="23" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="E19" s="23" t="s">
         <v>26</v>
       </c>
       <c r="F19" s="23" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="G19" s="23" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="H19" s="19">
         <v>1750736</v>
@@ -2407,19 +2398,19 @@
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="D20" s="23" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="E20" s="23" t="s">
         <v>12</v>
       </c>
       <c r="F20" s="23" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G20" s="23" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
       <c r="H20" s="19">
         <v>2059500</v>
@@ -2440,16 +2431,16 @@
         <v>2</v>
       </c>
       <c r="C21" s="23" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="D21" s="23" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
       <c r="E21" s="23" t="s">
         <v>26</v>
       </c>
       <c r="F21" s="23" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
       <c r="G21" s="23" t="s">
         <v>13</v>
@@ -2482,7 +2473,7 @@
     <row r="23" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A23" s="11"/>
       <c r="B23" s="17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="15"/>
@@ -2514,7 +2505,7 @@
         <v>29</v>
       </c>
       <c r="F24" s="24" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="G24" s="23" t="s">
         <v>30</v>
@@ -2549,7 +2540,7 @@
         <v>33</v>
       </c>
       <c r="F25" s="24" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="G25" s="23" t="s">
         <v>30</v>
@@ -2585,7 +2576,7 @@
         <v>33</v>
       </c>
       <c r="F26" s="24" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="G26" s="23" t="s">
         <v>36</v>
@@ -2620,7 +2611,7 @@
         <v>33</v>
       </c>
       <c r="F27" s="24" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="G27" s="23" t="s">
         <v>39</v>
@@ -2653,7 +2644,7 @@
         <v>33</v>
       </c>
       <c r="F28" s="24" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G28" s="23" t="s">
         <v>50</v>
@@ -2679,15 +2670,17 @@
       <c r="B29" s="19">
         <v>1</v>
       </c>
-      <c r="C29" s="23"/>
+      <c r="C29" s="23" t="s">
+        <v>140</v>
+      </c>
       <c r="D29" s="23" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="E29" s="23" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="G29" s="23" t="s">
         <v>50</v>
@@ -2713,18 +2706,20 @@
       <c r="B30" s="19">
         <v>2</v>
       </c>
-      <c r="C30" s="23"/>
+      <c r="C30" s="23" t="s">
+        <v>141</v>
+      </c>
       <c r="D30" s="23" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="E30" s="23">
         <v>1210</v>
       </c>
       <c r="F30" s="24" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="H30" s="19">
         <v>2449143</v>
@@ -2747,18 +2742,20 @@
       <c r="B31" s="19">
         <v>1</v>
       </c>
-      <c r="C31" s="23"/>
+      <c r="C31" s="23" t="s">
+        <v>142</v>
+      </c>
       <c r="D31" s="23" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="E31" s="23" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="F31" s="24" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="H31" s="19">
         <v>1759283</v>
@@ -2781,18 +2778,20 @@
       <c r="B32" s="19">
         <v>1</v>
       </c>
-      <c r="C32" s="23"/>
+      <c r="C32" s="23" t="s">
+        <v>147</v>
+      </c>
       <c r="D32" s="23" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="E32" s="23">
         <v>1812</v>
       </c>
       <c r="F32" s="24" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="G32" s="23" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="H32" s="19">
         <v>1702159</v>
@@ -2815,22 +2814,24 @@
       <c r="B33" s="19">
         <v>3</v>
       </c>
-      <c r="C33" s="23"/>
+      <c r="C33" s="23" t="s">
+        <v>151</v>
+      </c>
       <c r="D33" s="23" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="E33" s="23" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="F33" s="24" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="G33" s="23" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="H33" s="19"/>
       <c r="I33" s="19" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="J33" s="43"/>
       <c r="K33" s="30"/>
@@ -2863,7 +2864,7 @@
     <row r="35" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A35" s="11"/>
       <c r="B35" s="17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C35" s="15"/>
       <c r="D35" s="15"/>
@@ -2880,29 +2881,29 @@
     </row>
     <row r="36" spans="1:71" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="19" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="B36" s="19">
         <v>2</v>
       </c>
       <c r="C36" s="23" t="s">
-        <v>51</v>
+        <v>174</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E36" s="23" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="F36" s="24" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G36" s="23" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="H36" s="19"/>
       <c r="I36" s="19" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="J36" s="43"/>
       <c r="K36" s="30"/>
@@ -2919,19 +2920,19 @@
         <v>3</v>
       </c>
       <c r="C37" s="23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D37" s="23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E37" s="23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F37" s="24" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="G37" s="23" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H37" s="19">
         <v>1634758</v>
@@ -2946,25 +2947,25 @@
     </row>
     <row r="38" spans="1:71" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="19" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="B38" s="19">
         <v>2</v>
       </c>
       <c r="C38" s="23" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="D38" s="23" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E38" s="23" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="F38" s="23" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="G38" s="23" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H38" s="19">
         <v>1506642</v>
@@ -2985,19 +2986,19 @@
         <v>6</v>
       </c>
       <c r="C39" s="23" t="s">
-        <v>89</v>
+        <v>134</v>
       </c>
       <c r="D39" s="23" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E39" s="23" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="F39" s="23" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="G39" s="23" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="H39" s="19">
         <v>9604383</v>
@@ -3018,23 +3019,23 @@
         <v>4</v>
       </c>
       <c r="C40" s="23" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D40" s="23" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E40" s="23" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="F40" s="23" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="G40" s="23" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="H40" s="19"/>
       <c r="I40" s="19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="J40" s="43"/>
       <c r="K40" s="30"/>
@@ -3045,25 +3046,25 @@
     </row>
     <row r="41" spans="1:71" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="22" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B41" s="19">
         <v>2</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E41" s="23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="F41" s="23" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="G41" s="23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="H41" s="19">
         <v>1439485</v>
@@ -3087,20 +3088,20 @@
         <v>14</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="E42" s="23" t="s">
         <v>15</v>
       </c>
       <c r="F42" s="23" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="G42" s="23" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="H42" s="19"/>
       <c r="I42" s="19" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="J42" s="43"/>
       <c r="K42" s="30"/>
@@ -3116,18 +3117,20 @@
       <c r="B43" s="19">
         <v>1</v>
       </c>
-      <c r="C43" s="23"/>
+      <c r="C43" s="23" t="s">
+        <v>180</v>
+      </c>
       <c r="D43" s="23" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="E43" s="23" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
       <c r="F43" s="23" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="G43" s="23" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="H43" s="19">
         <v>2366012</v>
@@ -3157,7 +3160,7 @@
     <row r="45" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A45" s="11"/>
       <c r="B45" s="17" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C45" s="15"/>
       <c r="D45" s="15"/>
@@ -3180,19 +3183,19 @@
         <v>24</v>
       </c>
       <c r="C46" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="D46" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E46" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="D46" s="23" t="s">
+      <c r="F46" s="24" t="s">
+        <v>170</v>
+      </c>
+      <c r="G46" s="23" t="s">
         <v>65</v>
-      </c>
-      <c r="E46" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="F46" s="24" t="s">
-        <v>176</v>
-      </c>
-      <c r="G46" s="23" t="s">
-        <v>67</v>
       </c>
       <c r="H46" s="19">
         <v>2463562</v>
@@ -3214,16 +3217,16 @@
         <v>1</v>
       </c>
       <c r="C47" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="D47" s="23" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E47" s="23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F47" s="24" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="G47" s="23"/>
       <c r="H47" s="19">
@@ -3245,19 +3248,19 @@
         <v>2</v>
       </c>
       <c r="C48" s="23" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D48" s="23" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E48" s="23" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F48" s="24" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="G48" s="23" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H48" s="19">
         <v>2099223</v>
@@ -3278,19 +3281,19 @@
         <v>2</v>
       </c>
       <c r="C49" s="23" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D49" s="23" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E49" s="23" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="F49" s="23" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="G49" s="23" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="H49" s="19">
         <v>1837055</v>
@@ -3310,18 +3313,20 @@
       <c r="B50" s="28">
         <v>1</v>
       </c>
-      <c r="C50" s="29"/>
+      <c r="C50" s="29" t="s">
+        <v>157</v>
+      </c>
       <c r="D50" s="29" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="E50" s="29" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="F50" s="29" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="G50" s="29" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H50" s="28">
         <v>1713904</v>
@@ -3341,22 +3346,24 @@
       <c r="B51" s="28">
         <v>1</v>
       </c>
-      <c r="C51" s="29"/>
+      <c r="C51" s="29" t="s">
+        <v>164</v>
+      </c>
       <c r="D51" s="29" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="E51" s="29" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="F51" s="29" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="G51" s="29" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="H51" s="28"/>
       <c r="I51" s="28" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="J51" s="33"/>
       <c r="K51" s="33"/>
@@ -3372,18 +3379,20 @@
       <c r="B52" s="28">
         <v>3</v>
       </c>
-      <c r="C52" s="29"/>
+      <c r="C52" s="29" t="s">
+        <v>166</v>
+      </c>
       <c r="D52" s="29" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="E52" s="29" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="F52" s="29" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G52" s="29" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="H52" s="28">
         <v>1713889</v>
@@ -3411,7 +3420,7 @@
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
       <c r="B54" s="13" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
@@ -3430,19 +3439,19 @@
         <v>12</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D55" s="23" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F55" s="23" t="s">
-        <v>206</v>
+        <v>200</v>
       </c>
       <c r="G55" s="23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H55" s="19">
         <v>1894738</v>
@@ -3463,19 +3472,19 @@
         <v>2</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D56" s="23" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E56" s="23" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F56" s="23" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="G56" s="23" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="H56" s="19">
         <v>1829309</v>
@@ -3503,7 +3512,7 @@
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" s="12"/>
       <c r="B58" s="13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14"/>
@@ -3516,25 +3525,25 @@
     </row>
     <row r="59" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="19" t="s">
-        <v>198</v>
+        <v>192</v>
       </c>
       <c r="B59" s="19">
         <v>2</v>
       </c>
       <c r="C59" s="23" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D59" s="23" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="E59" s="23" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="F59" s="23" t="s">
-        <v>204</v>
+        <v>198</v>
       </c>
       <c r="G59" s="23" t="s">
-        <v>203</v>
+        <v>197</v>
       </c>
       <c r="H59" s="19"/>
       <c r="I59" s="19"/>
@@ -3547,27 +3556,29 @@
     </row>
     <row r="60" spans="1:15" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="19" t="s">
-        <v>205</v>
+        <v>199</v>
       </c>
       <c r="B60" s="19">
         <v>1</v>
       </c>
-      <c r="C60" s="23"/>
+      <c r="C60" s="23" t="s">
+        <v>193</v>
+      </c>
       <c r="D60" s="23" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E60" s="23" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="F60" s="23" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="G60" s="23" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="H60" s="19"/>
       <c r="I60" s="19" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="J60" s="43"/>
       <c r="K60" s="30"/>
@@ -3584,23 +3595,23 @@
         <v>6</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D61" s="23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E61" s="23" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="F61" s="24" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
       <c r="G61" s="23" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="H61" s="19"/>
       <c r="I61" s="19" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="J61" s="43"/>
       <c r="K61" s="30"/>
@@ -3617,19 +3628,19 @@
         <v>13</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="D62" s="23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E62" s="23" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="F62" s="24" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G62" s="23" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="H62" s="19">
         <v>9921826</v>
@@ -3659,10 +3670,10 @@
         <v>8</v>
       </c>
       <c r="F63" s="24" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="G63" s="23" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="H63" s="19">
         <v>1596919</v>
@@ -3682,18 +3693,20 @@
       <c r="B64" s="19">
         <v>1</v>
       </c>
-      <c r="C64" s="23"/>
+      <c r="C64" s="23" t="s">
+        <v>232</v>
+      </c>
       <c r="D64" s="23" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="E64" s="23" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="F64" s="24" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="G64" s="23" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="H64" s="19">
         <v>1596526</v>
@@ -3713,18 +3726,20 @@
       <c r="B65" s="19">
         <v>1</v>
       </c>
-      <c r="C65" s="23"/>
+      <c r="C65" s="23" t="s">
+        <v>188</v>
+      </c>
       <c r="D65" s="23" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="E65" s="23" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="F65" s="24" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="G65" s="23" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="H65" s="19">
         <v>2431496</v>
@@ -3752,7 +3767,7 @@
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A67" s="12"/>
       <c r="B67" s="13" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="C67" s="14"/>
       <c r="D67" s="14"/>
@@ -3771,19 +3786,19 @@
         <v>6</v>
       </c>
       <c r="C68" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="D68" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="E68" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="F68" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="G68" s="23" t="s">
         <v>56</v>
-      </c>
-      <c r="D68" s="23" t="s">
-        <v>56</v>
-      </c>
-      <c r="E68" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="F68" s="24" t="s">
-        <v>209</v>
-      </c>
-      <c r="G68" s="23" t="s">
-        <v>58</v>
       </c>
       <c r="H68" s="19">
         <v>1012251</v>
@@ -3804,19 +3819,19 @@
         <v>2</v>
       </c>
       <c r="C69" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D69" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E69" s="23" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F69" s="24" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="G69" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H69" s="19">
         <v>9961380</v>
@@ -3837,19 +3852,19 @@
         <v>1</v>
       </c>
       <c r="C70" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D70" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E70" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F70" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="D70" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="E70" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="F70" s="24" t="s">
-        <v>63</v>
-      </c>
       <c r="G70" s="23" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H70" s="19">
         <v>1012245</v>
@@ -3870,19 +3885,19 @@
         <v>2</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D71" s="23" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E71" s="23" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="F71" s="23" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G71" s="23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H71" s="19">
         <v>2578720</v>
@@ -3903,19 +3918,19 @@
         <v>2</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D72" s="23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="E72" s="23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="F72" s="23" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G72" s="23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H72" s="19">
         <v>2025256</v>
@@ -3936,19 +3951,19 @@
         <v>1</v>
       </c>
       <c r="C73" s="23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D73" s="23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E73" s="23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="F73" s="23" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="G73" s="23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H73" s="19">
         <v>2025257</v>
@@ -3968,18 +3983,20 @@
       <c r="B74" s="19">
         <v>1</v>
       </c>
-      <c r="C74" s="23"/>
+      <c r="C74" s="23" t="s">
+        <v>204</v>
+      </c>
       <c r="D74" s="23" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="E74" s="23" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="F74" s="23" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="G74" s="23" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="H74" s="19">
         <v>2025248</v>

</xml_diff>